<commit_message>
update year movie and net
</commit_message>
<xml_diff>
--- a/total_csv/Netflix_csv/Netflix.xlsx
+++ b/total_csv/Netflix_csv/Netflix.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\20205-lab\project\JJJJ_Project\Movie_XLSX\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\20205-lab\project\JJJJ_Project\total_csv\Netflix_csv\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2348C9EA-EFA0-4423-8641-6E4393102998}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC4BBE0F-E525-4266-8C47-B70B764DEB16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="22080" windowHeight="13176" xr2:uid="{6984766B-A560-4EE4-B7CF-463200AB2898}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="23070" windowHeight="13740" xr2:uid="{6984766B-A560-4EE4-B7CF-463200AB2898}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="36">
   <si>
     <t xml:space="preserve">구독자수 </t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -125,6 +125,50 @@
   </si>
   <si>
     <t xml:space="preserve">아시아태평양 매출액 증가률 </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Year </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Asia_sub</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Sub_growth </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Asia_revenue </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Movie_revenue </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Net_revenue_growth</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Movie_growth</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Audience</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Audience_growth</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Net_contents</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Movies</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -132,8 +176,12 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="177" formatCode="0.00_);[Red]\(0.00\)"/>
+  <numFmts count="5">
+    <numFmt numFmtId="176" formatCode="0.00_);[Red]\(0.00\)"/>
+    <numFmt numFmtId="177" formatCode="0_);[Red]\(0\)"/>
+    <numFmt numFmtId="178" formatCode="0_ "/>
+    <numFmt numFmtId="179" formatCode="0.00_ "/>
+    <numFmt numFmtId="180" formatCode="0.00;[Red]0.00"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -199,7 +247,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -215,11 +263,23 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -536,28 +596,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDB79F15-00E8-4EF1-857D-2387F8F1F49A}">
-  <dimension ref="A1:N26"/>
+  <dimension ref="A1:N36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.8984375" customWidth="1"/>
-    <col min="2" max="3" width="15.3984375" customWidth="1"/>
-    <col min="4" max="4" width="19.3984375" customWidth="1"/>
-    <col min="5" max="5" width="21.3984375" customWidth="1"/>
-    <col min="6" max="6" width="17.09765625" customWidth="1"/>
-    <col min="7" max="7" width="20.19921875" customWidth="1"/>
-    <col min="8" max="8" width="13.296875" customWidth="1"/>
-    <col min="9" max="9" width="15.296875" customWidth="1"/>
+    <col min="1" max="1" width="11.875" customWidth="1"/>
+    <col min="2" max="3" width="15.375" customWidth="1"/>
+    <col min="4" max="4" width="19.375" customWidth="1"/>
+    <col min="5" max="5" width="21.375" customWidth="1"/>
+    <col min="6" max="6" width="17.25" customWidth="1"/>
+    <col min="7" max="7" width="20.25" customWidth="1"/>
+    <col min="8" max="8" width="13.25" customWidth="1"/>
+    <col min="9" max="9" width="15.25" customWidth="1"/>
     <col min="10" max="10" width="16.5" customWidth="1"/>
-    <col min="11" max="12" width="11.09765625" customWidth="1"/>
-    <col min="15" max="15" width="15.8984375" customWidth="1"/>
+    <col min="11" max="12" width="11.125" customWidth="1"/>
+    <col min="15" max="15" width="15.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>12</v>
       </c>
@@ -589,7 +649,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>2</v>
       </c>
@@ -618,7 +678,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>3</v>
       </c>
@@ -650,7 +710,7 @@
         <v>9.0625</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>4</v>
       </c>
@@ -682,7 +742,7 @@
         <v>9.455587392550143</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>5</v>
       </c>
@@ -714,7 +774,7 @@
         <v>9.4240837696335085</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>6</v>
       </c>
@@ -746,7 +806,7 @@
         <v>15.789473684210526</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
         <v>7</v>
       </c>
@@ -778,7 +838,7 @@
         <v>17.561983471074381</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>8</v>
       </c>
@@ -810,7 +870,7 @@
         <v>11.599297012302284</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
         <v>9</v>
       </c>
@@ -842,7 +902,7 @@
         <v>7.8740157480314963</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
         <v>10</v>
       </c>
@@ -874,7 +934,7 @@
         <v>11.240875912408759</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="5"/>
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
@@ -885,7 +945,7 @@
       <c r="H11" s="5"/>
       <c r="I11" s="5"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="5"/>
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
@@ -896,7 +956,7 @@
       <c r="H12" s="5"/>
       <c r="I12" s="5"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="5"/>
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
@@ -907,7 +967,7 @@
       <c r="H13" s="5"/>
       <c r="I13" s="5"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" s="5"/>
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
@@ -918,7 +978,7 @@
       <c r="H14" s="5"/>
       <c r="I14" s="5"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" s="5"/>
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
@@ -929,7 +989,7 @@
       <c r="H15" s="5"/>
       <c r="I15" s="5"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" s="5" t="s">
         <v>13</v>
       </c>
@@ -958,8 +1018,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="A17" s="5">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A17" s="7">
         <v>2019</v>
       </c>
       <c r="B17" s="5">
@@ -985,8 +1045,8 @@
       </c>
       <c r="I17" s="5"/>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="A18" s="5">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A18" s="7">
         <v>2020</v>
       </c>
       <c r="B18" s="5">
@@ -1015,12 +1075,17 @@
       </c>
       <c r="I18" s="5"/>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>13</v>
       </c>
@@ -1028,29 +1093,184 @@
         <v>16</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>2019</v>
       </c>
       <c r="B24" s="2">
         <v>5769</v>
       </c>
-    </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.4">
+      <c r="E24">
+        <v>1948</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>2020</v>
       </c>
       <c r="B25" s="2">
         <v>5838</v>
+      </c>
+      <c r="E25">
+        <v>1899</v>
       </c>
       <c r="F25" s="4"/>
       <c r="L25" s="1"/>
       <c r="M25" s="1"/>
       <c r="N25" s="3"/>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
       <c r="M26" s="1"/>
       <c r="N26" s="1"/>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="F27">
+        <v>1913989080068</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A30" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D30" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E30" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F30" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="G30" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="H30" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="I30" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="J30" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="K30" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A31" s="7">
+        <v>2019</v>
+      </c>
+      <c r="B31" s="5">
+        <v>55.8</v>
+      </c>
+      <c r="C31" s="5"/>
+      <c r="D31" s="5">
+        <v>1469</v>
+      </c>
+      <c r="E31" s="5"/>
+      <c r="F31" s="2">
+        <v>5769</v>
+      </c>
+      <c r="G31" s="9">
+        <v>1913989.08</v>
+      </c>
+      <c r="H31" s="8"/>
+      <c r="I31" s="10">
+        <v>226.678777</v>
+      </c>
+      <c r="K31">
+        <v>1948</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A32" s="7">
+        <v>2020</v>
+      </c>
+      <c r="B32" s="5">
+        <v>91.32</v>
+      </c>
+      <c r="C32" s="5">
+        <f>(B32-B31)/B31*100</f>
+        <v>63.655913978494617</v>
+      </c>
+      <c r="D32" s="5">
+        <v>2373</v>
+      </c>
+      <c r="E32" s="5">
+        <f>(D32-D31)/D31*100</f>
+        <v>61.53846153846154</v>
+      </c>
+      <c r="F32" s="2">
+        <v>5838</v>
+      </c>
+      <c r="G32" s="9">
+        <v>510375.22219100001</v>
+      </c>
+      <c r="H32" s="9">
+        <v>-73</v>
+      </c>
+      <c r="I32" s="10">
+        <v>59.524093000000001</v>
+      </c>
+      <c r="J32" s="9">
+        <v>-74</v>
+      </c>
+      <c r="K32">
+        <v>1899</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A35" s="7">
+        <v>2019</v>
+      </c>
+      <c r="B35" s="5">
+        <v>55.8</v>
+      </c>
+      <c r="C35" s="5">
+        <v>1469</v>
+      </c>
+      <c r="D35" s="2">
+        <v>5769</v>
+      </c>
+      <c r="E35" s="9">
+        <v>1913989.08</v>
+      </c>
+      <c r="F35" s="10">
+        <v>226.678777</v>
+      </c>
+      <c r="G35">
+        <v>1948</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A36" s="7">
+        <v>2020</v>
+      </c>
+      <c r="B36" s="5">
+        <v>91.32</v>
+      </c>
+      <c r="C36" s="5">
+        <v>2373</v>
+      </c>
+      <c r="D36" s="2">
+        <v>5838</v>
+      </c>
+      <c r="E36" s="9">
+        <v>510375.22219100001</v>
+      </c>
+      <c r="F36" s="10">
+        <v>59.524093000000001</v>
+      </c>
+      <c r="G36">
+        <v>1899</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
update conf and csv
</commit_message>
<xml_diff>
--- a/total_csv/Netflix_csv/Netflix.xlsx
+++ b/total_csv/Netflix_csv/Netflix.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\20205-lab\project\JJJJ_Project\total_csv\Netflix_csv\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D6D6386-D230-4F77-B4D7-715A2FC9B8B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7614E9CC-E5B7-430E-AC63-4D9E701AFC1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="23070" windowHeight="13740" xr2:uid="{6984766B-A560-4EE4-B7CF-463200AB2898}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="37">
   <si>
     <t xml:space="preserve">구독자수 </t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -169,6 +169,10 @@
   </si>
   <si>
     <t>Movies</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Net_sub_growth </t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -596,10 +600,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDB79F15-00E8-4EF1-857D-2387F8F1F49A}">
-  <dimension ref="A1:N36"/>
+  <dimension ref="A1:N40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="E39" sqref="E39"/>
+    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="I41" sqref="I41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1295,6 +1299,40 @@
         <v>1899</v>
       </c>
     </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A39" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B39" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C39" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D39" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="E39" s="5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A40" s="7">
+        <v>2020</v>
+      </c>
+      <c r="B40" s="5">
+        <v>64</v>
+      </c>
+      <c r="C40" s="9">
+        <v>62</v>
+      </c>
+      <c r="D40" s="9">
+        <v>-73</v>
+      </c>
+      <c r="E40" s="9">
+        <v>-74</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>